<commit_message>
error throwback as file
</commit_message>
<xml_diff>
--- a/(BE Request)Database Template for Residency (1).xlsx
+++ b/(BE Request)Database Template for Residency (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maarunipandithurai/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09595E7D-3731-3D40-8E5D-E629CDB5A8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96BAF63-9647-C84A-AB38-6D77D3328A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="3920" windowWidth="29040" windowHeight="15720" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal Details" sheetId="11" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="516">
   <si>
     <t>Employee ID/ MOHH Employee No</t>
   </si>
@@ -1623,6 +1623,15 @@
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>nannn</t>
+  </si>
+  <si>
+    <t>lkjlj</t>
+  </si>
+  <si>
+    <t>kjhojlkjl</t>
   </si>
 </sst>
 </file>
@@ -6729,7 +6738,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="9" topLeftCell="AA1" activePane="topRight" state="frozen"/>
       <selection activeCell="O23" sqref="O23"/>
-      <selection pane="topRight" activeCell="AA14" sqref="AA14"/>
+      <selection pane="topRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7832,57 +7841,66 @@
       </c>
     </row>
     <row r="15" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>513</v>
+      </c>
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>514</v>
+      </c>
       <c r="M16" s="20"/>
     </row>
-    <row r="17" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>515</v>
+      </c>
       <c r="M17" s="20"/>
     </row>
-    <row r="18" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M18" s="20"/>
     </row>
-    <row r="19" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M19" s="20"/>
     </row>
-    <row r="20" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M20" s="20"/>
     </row>
-    <row r="21" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M22" s="20"/>
     </row>
-    <row r="23" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M23" s="20"/>
     </row>
-    <row r="24" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M24" s="20"/>
     </row>
-    <row r="25" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M25" s="20"/>
     </row>
-    <row r="26" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M26" s="20"/>
     </row>
-    <row r="27" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M27" s="20"/>
     </row>
-    <row r="28" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M28" s="20"/>
     </row>
-    <row r="29" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M29" s="20"/>
     </row>
-    <row r="30" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M30" s="20"/>
     </row>
-    <row r="31" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M31" s="20"/>
     </row>
-    <row r="32" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M32" s="20"/>
     </row>
     <row r="33" spans="13:13" s="15" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>